<commit_message>
fix: weekly fake-data was not rendered correctly
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_0/1_0_weekly_repeated.xlsx
+++ b/R/data/dictionaries/outcome/1_0/1_0_weekly_repeated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD242D0-CEF5-4341-BF58-26903B63C3A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D298BEF3-BB74-4045-9AB3-103576E2123D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,58 +56,28 @@
     <t>m_sbp_</t>
   </si>
   <si>
-    <t>mother's systolic blood pressure during pregnancy in completed weeks of gestation</t>
-  </si>
-  <si>
     <t>m_dbp_</t>
-  </si>
-  <si>
-    <t>mother's diastolic blood pressure during pregnancy in completed weeks of gestation</t>
   </si>
   <si>
     <t>m_crp_</t>
   </si>
   <si>
-    <t>mother's CRP during pregnancy in completed weeks of gestation</t>
-  </si>
-  <si>
     <t>m_glucose_</t>
-  </si>
-  <si>
-    <t>mother's glucose during pregnancy in completed weeks of gestation</t>
   </si>
   <si>
     <t>m_haem_</t>
   </si>
   <si>
-    <t>mother's haemoglobin during pregnancy in completed weeks of gestation</t>
-  </si>
-  <si>
     <t>m_hba1c_</t>
-  </si>
-  <si>
-    <t>mother's HbA1c during pregnancy in completed weeks of gestation</t>
   </si>
   <si>
     <t>m_insulin_</t>
   </si>
   <si>
-    <t>mother's insulin during pregnancy in completed weeks of gestation</t>
-  </si>
-  <si>
     <t>m_hdlc_</t>
   </si>
   <si>
-    <t>mother's HDLc during pregnancy in completed weeks of gestation</t>
-  </si>
-  <si>
     <t>m_ldlc_</t>
-  </si>
-  <si>
-    <t>mother's LDLc during pregnancy in completed weeks of gestation</t>
-  </si>
-  <si>
-    <t>mother's total cholesterol during pregnancy in completed weeks of gestation</t>
   </si>
   <si>
     <t>m_chol_</t>
@@ -123,12 +93,6 @@
   </si>
   <si>
     <t>f_dbp_</t>
-  </si>
-  <si>
-    <t>father's systolic blood pressure during pregnancy in completed weeks of gestation</t>
-  </si>
-  <si>
-    <t>father's diastolic blood pressure during pregnancy in completed weeks of gestation</t>
   </si>
   <si>
     <t>row_id</t>
@@ -162,6 +126,42 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>Mother's systolic blood pressure during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's diastolic blood pressure during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's CRP during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's glucose during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's haemoglobin during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's HbA1c during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's insulin during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's HDLc during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's LDLc during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Mother's total cholesterol during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Father's systolic blood pressure during pregnancy in completed weeks of gestation</t>
+  </si>
+  <si>
+    <t>Father's diastolic blood pressure during pregnancy in completed weeks of gestation</t>
   </si>
 </sst>
 </file>
@@ -746,7 +746,7 @@
   <dimension ref="A1:BG142"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -829,16 +829,16 @@
     </row>
     <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -898,14 +898,14 @@
     </row>
     <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -965,16 +965,16 @@
     </row>
     <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -1034,16 +1034,16 @@
     </row>
     <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -1112,7 +1112,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>4</v>
@@ -1181,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>4</v>
@@ -1250,13 +1250,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>4</v>
@@ -1265,13 +1265,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>4</v>
@@ -1280,13 +1280,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>4</v>
@@ -1295,13 +1295,13 @@
         <v>5</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>4</v>
@@ -1310,13 +1310,13 @@
         <v>5</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>4</v>
@@ -1325,13 +1325,13 @@
         <v>7</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>4</v>
@@ -1340,13 +1340,13 @@
         <v>5</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>4</v>
@@ -1355,13 +1355,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>4</v>
@@ -1370,13 +1370,13 @@
         <v>5</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>4</v>
@@ -1385,13 +1385,13 @@
         <v>5</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>4</v>
@@ -1400,13 +1400,13 @@
         <v>6</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>4</v>
@@ -1415,7 +1415,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E19" s="15"/>
     </row>

</xml_diff>